<commit_message>
stock market example revised (need to do: price -> float)
</commit_message>
<xml_diff>
--- a/tutorial/StockMarket/data/input/simulator_scenarios.xlsx
+++ b/tutorial/StockMarket/data/input/simulator_scenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/ABM4ALL/Melodie/tutorial/StockMarket/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF478CDC-5FE9-6B4F-B120-333CBED1B7B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E391FDC4-4755-1A4D-8CD3-80CDE4D56D9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3600" yWindow="760" windowWidth="23400" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,9 +64,6 @@
     <t>chartist_percentage_start</t>
   </si>
   <si>
-    <t>forecast_rule_evaluation_memory</t>
-  </si>
-  <si>
     <t>stock_trading_volume</t>
   </si>
   <si>
@@ -74,6 +71,9 @@
   </si>
   <si>
     <t>cash_account_start</t>
+  </si>
+  <si>
+    <t>forecast_rule_evaluation_memory_length</t>
   </si>
 </sst>
 </file>
@@ -397,7 +397,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="181" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -444,7 +444,7 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>7</v>
@@ -453,13 +453,13 @@
         <v>8</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
stock example simulation setup
</commit_message>
<xml_diff>
--- a/tutorial/StockMarket/data/input/simulator_scenarios.xlsx
+++ b/tutorial/StockMarket/data/input/simulator_scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/ABM4ALL/Melodie/tutorial/StockMarket/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E391FDC4-4755-1A4D-8CD3-80CDE4D56D9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75ABBAB-A022-CF45-8AB1-D2ED9F13450E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="760" windowWidth="23400" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="760" windowWidth="26880" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="simulator_scenarios" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>id</t>
   </si>
@@ -49,21 +49,9 @@
     <t>period_ticks</t>
   </si>
   <si>
-    <t>chartist_memory_length</t>
-  </si>
-  <si>
-    <t>fundamentalist_price_benchmark</t>
-  </si>
-  <si>
-    <t>switch_intensity</t>
-  </si>
-  <si>
     <t>stock_price_start</t>
   </si>
   <si>
-    <t>chartist_percentage_start</t>
-  </si>
-  <si>
     <t>stock_trading_volume</t>
   </si>
   <si>
@@ -73,14 +61,32 @@
     <t>cash_account_start</t>
   </si>
   <si>
-    <t>forecast_rule_evaluation_memory_length</t>
+    <t>chartist_forecast_start_min</t>
+  </si>
+  <si>
+    <t>chartist_forecast_start_max</t>
+  </si>
+  <si>
+    <t>fundamentalist_forecast_min</t>
+  </si>
+  <si>
+    <t>fundamentalist_forecast_max</t>
+  </si>
+  <si>
+    <t>chartist_forecast_memory_length</t>
+  </si>
+  <si>
+    <t>fundamentalist_weight_min</t>
+  </si>
+  <si>
+    <t>fundamentalist_weight_max</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,6 +100,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val=".AppleSystemUIFont"/>
     </font>
   </fonts>
   <fills count="2">
@@ -116,9 +127,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,31 +407,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="181" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="181" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" customWidth="1"/>
     <col min="3" max="3" width="7.1640625" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.1640625" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="20.83203125" customWidth="1"/>
+    <col min="12" max="12" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -435,34 +447,40 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16">
       <c r="A2">
         <v>0</v>
       </c>
@@ -479,32 +497,44 @@
         <v>1000</v>
       </c>
       <c r="F2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I2">
-        <v>5</v>
-      </c>
-      <c r="J2" s="1">
-        <v>0.5</v>
+        <v>120</v>
+      </c>
+      <c r="J2">
+        <v>80</v>
       </c>
       <c r="K2">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M2">
         <v>100</v>
       </c>
       <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>100</v>
+      </c>
+      <c r="P2">
         <v>10000</v>
       </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="F6" s="2"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>